<commit_message>
fix: update blank sheet structure
</commit_message>
<xml_diff>
--- a/docs/blank-naturalist-spreadsheet.xlsx
+++ b/docs/blank-naturalist-spreadsheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\xampp\htdocs\naturalist\src\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programy\web\naturalist\naturalist\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B470D2-4B2E-4751-8D9E-106333803EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="6" r:id="rId1"/>
@@ -29,26 +30,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Dominik M. Ramík</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -77,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="118">
   <si>
     <t>Maps</t>
   </si>
@@ -453,11 +445,32 @@
   <si>
     <t>FAM</t>
   </si>
+  <si>
+    <t>Italicize</t>
+  </si>
+  <si>
+    <t>Parent taxon indication</t>
+  </si>
+  <si>
+    <t>Precache</t>
+  </si>
+  <si>
+    <t>Citations</t>
+  </si>
+  <si>
+    <t>In-text citation</t>
+  </si>
+  <si>
+    <t>Reference entry</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -643,13 +656,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -727,12 +741,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal 1" xfId="2"/>
+  <cellStyles count="5">
+    <cellStyle name="Excel Built-in Normal 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
+    <cellStyle name="Hypertextový odkaz 2" xfId="4" xr:uid="{E64F7537-A568-4A3E-9A72-A1A5152876BB}"/>
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
-    <cellStyle name="Normální 2" xfId="3"/>
+    <cellStyle name="Normální 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1147,10 +1185,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15"/>
   <cols>
@@ -1325,13 +1363,13 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:CY13248">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:CY13248">
     <sortCondition ref="B5:B13248"/>
     <sortCondition ref="C5:C13248"/>
     <sortCondition ref="E5:E13248"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -1339,7 +1377,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1565,82 +1603,96 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AG63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="29" customWidth="1"/>
-    <col min="19" max="19" width="4" customWidth="1"/>
-    <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18" customWidth="1"/>
-    <col min="22" max="22" width="21.7109375" customWidth="1"/>
-    <col min="23" max="23" width="25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="4" customWidth="1"/>
-    <col min="25" max="25" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="4" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18" customWidth="1"/>
+    <col min="25" max="25" width="21.7109375" customWidth="1"/>
+    <col min="26" max="26" width="25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4" customWidth="1"/>
+    <col min="28" max="28" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="4" style="46" customWidth="1"/>
+    <col min="31" max="31" width="15.7109375" style="46" customWidth="1"/>
+    <col min="32" max="32" width="46" style="46" customWidth="1"/>
+    <col min="33" max="33" width="15.85546875" style="46" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:33">
       <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="13"/>
+      <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="13"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="6" t="s">
+      <c r="N1" s="7"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="6" t="s">
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="6" t="s">
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="7"/>
-    </row>
-    <row r="2" spans="1:26" s="28" customFormat="1">
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+    </row>
+    <row r="2" spans="1:33" s="28" customFormat="1">
       <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
@@ -1650,109 +1702,135 @@
       <c r="C2" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="26" t="s">
+        <v>111</v>
+      </c>
       <c r="E2" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="H2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="I2" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="J2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="K2" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="L2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="26" t="s">
+      <c r="M2" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="N2" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="26" t="s">
+      <c r="P2" s="27"/>
+      <c r="Q2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="R2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="S2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="T2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="26" t="s">
+      <c r="U2" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="V2" s="27"/>
+      <c r="W2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="X2" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="Y2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="26" t="s">
+      <c r="Z2" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="26" t="s">
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="Z2" s="26" t="s">
+      <c r="AC2" s="26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:26">
+      <c r="AD2" s="40"/>
+      <c r="AE2" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF2" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG2" s="41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
       <c r="A3" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="H3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="24"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="24"/>
-      <c r="Z3" s="4"/>
-    </row>
-    <row r="4" spans="1:26">
+      <c r="V3" s="11"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="24"/>
+      <c r="AC3" s="4"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="43"/>
+      <c r="AF3" s="44"/>
+      <c r="AG3" s="44"/>
+    </row>
+    <row r="4" spans="1:33">
       <c r="A4" s="8" t="s">
         <v>110</v>
       </c>
@@ -1760,547 +1838,674 @@
         <v>52</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="I4" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="11"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="24"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="2"/>
-    </row>
-    <row r="5" spans="1:26">
+      <c r="V4" s="11"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="24"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="44"/>
+      <c r="AG4" s="44"/>
+    </row>
+    <row r="5" spans="1:33">
       <c r="A5" s="8" t="s">
         <v>54</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="1" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="24"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="14"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="24"/>
-      <c r="Z5" s="2"/>
-    </row>
-    <row r="6" spans="1:26">
+      <c r="V5" s="11"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="14"/>
+      <c r="AA5" s="11"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="42"/>
+      <c r="AE5" s="43"/>
+      <c r="AF5" s="44"/>
+      <c r="AG5" s="45"/>
+    </row>
+    <row r="6" spans="1:33">
       <c r="A6" s="8" t="s">
         <v>55</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="1" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="11"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="2"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="11"/>
       <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="V6" s="11"/>
       <c r="W6" s="2"/>
-      <c r="X6" s="11"/>
-    </row>
-    <row r="7" spans="1:26">
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="11"/>
+      <c r="AD6" s="42"/>
+      <c r="AE6" s="44"/>
+      <c r="AF6" s="44"/>
+      <c r="AG6" s="44"/>
+    </row>
+    <row r="7" spans="1:33">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="1" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H7" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="8" t="s">
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="15"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="4"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:26">
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="42"/>
+      <c r="AE7" s="44"/>
+      <c r="AF7" s="44"/>
+      <c r="AG7" s="44"/>
+    </row>
+    <row r="8" spans="1:33">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-    </row>
-    <row r="9" spans="1:26">
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="42"/>
+      <c r="AE8" s="44"/>
+      <c r="AF8" s="44"/>
+      <c r="AG8" s="44"/>
+    </row>
+    <row r="9" spans="1:33">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="17"/>
       <c r="Q9" s="15"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="14"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="V9" s="11"/>
       <c r="W9" s="2"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="14"/>
       <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:26">
+      <c r="AA9" s="11"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="42"/>
+      <c r="AE9" s="44"/>
+      <c r="AF9" s="44"/>
+      <c r="AG9" s="45"/>
+    </row>
+    <row r="10" spans="1:33">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="24"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
-      <c r="N10" s="11"/>
+      <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="P10" s="11"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="11"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
       <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="11"/>
       <c r="W10" s="2"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="2"/>
+      <c r="X10" s="2"/>
       <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:26">
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="42"/>
+      <c r="AE10" s="44"/>
+      <c r="AF10" s="44"/>
+    </row>
+    <row r="11" spans="1:33">
       <c r="A11" s="2"/>
       <c r="B11" s="15"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
-      <c r="N11" s="11"/>
+      <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
+      <c r="P11" s="11"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="11"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
       <c r="T11" s="2"/>
-      <c r="U11" s="15"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="11"/>
       <c r="W11" s="2"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="15"/>
+      <c r="X11" s="15"/>
       <c r="Z11" s="2"/>
-    </row>
-    <row r="12" spans="1:26">
+      <c r="AA11" s="11"/>
+      <c r="AB11" s="15"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="42"/>
+      <c r="AE11" s="44"/>
+      <c r="AF11" s="47"/>
+    </row>
+    <row r="12" spans="1:33">
       <c r="A12" s="2"/>
       <c r="B12" s="15"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="24"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
-      <c r="N12" s="11"/>
+      <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
+      <c r="P12" s="11"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="11"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
       <c r="T12" s="2"/>
-      <c r="U12" s="15"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="11"/>
       <c r="W12" s="2"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="2"/>
+      <c r="X12" s="15"/>
       <c r="Z12" s="2"/>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="AA12" s="11"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="42"/>
+      <c r="AE12" s="44"/>
+      <c r="AF12" s="47"/>
+    </row>
+    <row r="13" spans="1:33">
       <c r="A13" s="2"/>
       <c r="B13" s="15"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
-      <c r="N13" s="11"/>
+      <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
+      <c r="P13" s="11"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="11"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
       <c r="T13" s="2"/>
-      <c r="U13" s="15"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="11"/>
       <c r="W13" s="2"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="15"/>
+      <c r="X13" s="15"/>
       <c r="Z13" s="2"/>
-    </row>
-    <row r="14" spans="1:26">
+      <c r="AA13" s="11"/>
+      <c r="AB13" s="15"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="42"/>
+      <c r="AE13" s="44"/>
+      <c r="AF13" s="47"/>
+    </row>
+    <row r="14" spans="1:33">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="11"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
+      <c r="P14" s="11"/>
       <c r="Q14" s="2"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="11"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
       <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
+      <c r="U14" s="24"/>
+      <c r="V14" s="11"/>
       <c r="W14" s="2"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="2"/>
+      <c r="X14" s="2"/>
       <c r="Z14" s="2"/>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="42"/>
+      <c r="AE14" s="44"/>
+      <c r="AF14" s="44"/>
+    </row>
+    <row r="15" spans="1:33">
       <c r="A15" s="2"/>
       <c r="B15" s="15"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="11"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="P15" s="11"/>
       <c r="Q15" s="2"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="11"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
       <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="11"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="2"/>
+      <c r="X15" s="2"/>
       <c r="Z15" s="2"/>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="AA15" s="11"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="42"/>
+      <c r="AE15" s="44"/>
+      <c r="AF15" s="44"/>
+    </row>
+    <row r="16" spans="1:33">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="11"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="P16" s="11"/>
       <c r="Q16" s="2"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="11"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
       <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="11"/>
       <c r="W16" s="2"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="2"/>
+      <c r="X16" s="2"/>
       <c r="Z16" s="2"/>
-    </row>
-    <row r="17" spans="1:26">
+      <c r="AA16" s="11"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="42"/>
+      <c r="AE16" s="44"/>
+      <c r="AF16" s="44"/>
+    </row>
+    <row r="17" spans="1:33">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="11"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="P17" s="11"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="11"/>
+      <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
+      <c r="V17" s="11"/>
       <c r="W17" s="2"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="2"/>
+      <c r="X17" s="2"/>
       <c r="Z17" s="2"/>
-    </row>
-    <row r="18" spans="1:26">
+      <c r="AA17" s="11"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="42"/>
+      <c r="AE17" s="44"/>
+      <c r="AF17" s="44"/>
+    </row>
+    <row r="18" spans="1:33">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="11"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="P18" s="11"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="11"/>
+      <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
+      <c r="V18" s="11"/>
       <c r="W18" s="2"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="2"/>
+      <c r="X18" s="2"/>
       <c r="Z18" s="2"/>
-    </row>
-    <row r="19" spans="1:26">
+      <c r="AA18" s="11"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="42"/>
+      <c r="AE18" s="44"/>
+      <c r="AF18" s="44"/>
+    </row>
+    <row r="19" spans="1:33">
       <c r="A19" s="2"/>
       <c r="B19" s="15"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-      <c r="N19" s="11"/>
+      <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="P19" s="11"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="11"/>
+      <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
+      <c r="V19" s="11"/>
       <c r="W19" s="2"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="2"/>
+      <c r="X19" s="2"/>
       <c r="Z19" s="2"/>
-    </row>
-    <row r="20" spans="1:26">
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="42"/>
+      <c r="AE19" s="44"/>
+      <c r="AF19" s="44"/>
+    </row>
+    <row r="20" spans="1:33">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="24"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="P20" s="11"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="11"/>
+      <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
+      <c r="V20" s="11"/>
       <c r="W20" s="2"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="2"/>
+      <c r="X20" s="2"/>
       <c r="Z20" s="2"/>
-    </row>
-    <row r="21" spans="1:26">
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="42"/>
+      <c r="AE20" s="44"/>
+      <c r="AF20" s="44"/>
+    </row>
+    <row r="21" spans="1:33">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="24"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="P21" s="11"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="11"/>
+      <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
+      <c r="V21" s="11"/>
       <c r="W21" s="2"/>
-      <c r="X21" s="11"/>
+      <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
-    </row>
-    <row r="22" spans="1:26">
+      <c r="AA21" s="11"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="42"/>
+      <c r="AE21" s="44"/>
+      <c r="AF21" s="44"/>
+      <c r="AG21" s="44"/>
+    </row>
+    <row r="22" spans="1:33">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="24"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="N22" s="11"/>
+      <c r="N22" s="2"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="P22" s="11"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="11"/>
+      <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
+      <c r="V22" s="11"/>
       <c r="W22" s="2"/>
-      <c r="X22" s="11"/>
+      <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
-    </row>
-    <row r="23" spans="1:26">
+      <c r="AA22" s="11"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="42"/>
+      <c r="AE22" s="44"/>
+      <c r="AF22" s="44"/>
+      <c r="AG22" s="44"/>
+    </row>
+    <row r="23" spans="1:33">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="24"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-      <c r="N23" s="11"/>
+      <c r="N23" s="2"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="P23" s="11"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="11"/>
+      <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
-      <c r="V23" s="2"/>
+      <c r="V23" s="11"/>
       <c r="W23" s="2"/>
-      <c r="X23" s="11"/>
+      <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
-      <c r="Z23" s="15"/>
-    </row>
-    <row r="24" spans="1:26">
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="15"/>
+      <c r="AD23" s="42"/>
+      <c r="AE23" s="44"/>
+      <c r="AF23" s="44"/>
+      <c r="AG23" s="44"/>
+    </row>
+    <row r="24" spans="1:33">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="11"/>
+      <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -2308,27 +2513,34 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
-      <c r="N24" s="11"/>
+      <c r="N24" s="2"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
+      <c r="P24" s="11"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="11"/>
+      <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
-      <c r="V24" s="2"/>
+      <c r="V24" s="11"/>
       <c r="W24" s="2"/>
-      <c r="X24" s="11"/>
+      <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-      <c r="Z24" s="15"/>
-    </row>
-    <row r="25" spans="1:26">
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="15"/>
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="44"/>
+      <c r="AF24" s="44"/>
+      <c r="AG24" s="44"/>
+    </row>
+    <row r="25" spans="1:33">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="11"/>
+      <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -2336,27 +2548,34 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
-      <c r="N25" s="11"/>
+      <c r="N25" s="2"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="2"/>
+      <c r="P25" s="11"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="11"/>
+      <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
+      <c r="V25" s="11"/>
       <c r="W25" s="2"/>
-      <c r="X25" s="11"/>
+      <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
-      <c r="Z25" s="15"/>
-    </row>
-    <row r="26" spans="1:26">
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="15"/>
+      <c r="AD25" s="42"/>
+      <c r="AE25" s="44"/>
+      <c r="AF25" s="44"/>
+      <c r="AG25" s="44"/>
+    </row>
+    <row r="26" spans="1:33">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="11"/>
+      <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -2364,148 +2583,190 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
-      <c r="N26" s="11"/>
+      <c r="N26" s="2"/>
       <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
+      <c r="P26" s="11"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="11"/>
+      <c r="S26" s="2"/>
       <c r="T26" s="2"/>
       <c r="U26" s="2"/>
-      <c r="V26" s="2"/>
+      <c r="V26" s="11"/>
       <c r="W26" s="2"/>
-      <c r="X26" s="11"/>
+      <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
-    </row>
-    <row r="27" spans="1:26">
+      <c r="AA26" s="11"/>
+      <c r="AB26" s="2"/>
+      <c r="AC26" s="2"/>
+      <c r="AD26" s="42"/>
+      <c r="AE26" s="44"/>
+      <c r="AF26" s="44"/>
+      <c r="AG26" s="44"/>
+    </row>
+    <row r="27" spans="1:33">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="11"/>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="P27" s="11"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="11"/>
+      <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
-      <c r="V27" s="2"/>
+      <c r="V27" s="11"/>
       <c r="W27" s="2"/>
-      <c r="X27" s="11"/>
+      <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
-    </row>
-    <row r="28" spans="1:26">
+      <c r="AA27" s="11"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="42"/>
+      <c r="AE27" s="44"/>
+      <c r="AF27" s="44"/>
+      <c r="AG27" s="44"/>
+    </row>
+    <row r="28" spans="1:33">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="11"/>
+      <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="2"/>
-      <c r="P28" s="2"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="2"/>
+      <c r="P28" s="11"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="11"/>
+      <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
-      <c r="V28" s="2"/>
+      <c r="V28" s="11"/>
       <c r="W28" s="2"/>
-      <c r="X28" s="11"/>
+      <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
-    </row>
-    <row r="29" spans="1:26">
+      <c r="AA28" s="11"/>
+      <c r="AB28" s="2"/>
+      <c r="AC28" s="2"/>
+      <c r="AD28" s="42"/>
+      <c r="AE28" s="44"/>
+      <c r="AF28" s="44"/>
+      <c r="AG28" s="44"/>
+    </row>
+    <row r="29" spans="1:33">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="11"/>
+      <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
-      <c r="N29" s="11"/>
+      <c r="N29" s="2"/>
       <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
+      <c r="P29" s="11"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="11"/>
+      <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
-      <c r="V29" s="2"/>
+      <c r="V29" s="11"/>
       <c r="W29" s="2"/>
-      <c r="X29" s="11"/>
+      <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
-    </row>
-    <row r="30" spans="1:26">
+      <c r="AA29" s="11"/>
+      <c r="AB29" s="2"/>
+      <c r="AC29" s="2"/>
+      <c r="AD29" s="42"/>
+      <c r="AE29" s="44"/>
+      <c r="AF29" s="44"/>
+      <c r="AG29" s="44"/>
+    </row>
+    <row r="30" spans="1:33">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="11"/>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
       <c r="M30" s="2"/>
-      <c r="N30" s="11"/>
+      <c r="N30" s="2"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
+      <c r="P30" s="11"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="11"/>
+      <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
-      <c r="V30" s="2"/>
+      <c r="V30" s="11"/>
       <c r="W30" s="2"/>
-      <c r="X30" s="11"/>
+      <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
-    </row>
-    <row r="31" spans="1:26">
+      <c r="AA30" s="11"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="42"/>
+      <c r="AE30" s="44"/>
+      <c r="AF30" s="44"/>
+      <c r="AG30" s="44"/>
+    </row>
+    <row r="31" spans="1:33">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="11"/>
+      <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
-      <c r="N31" s="11"/>
+      <c r="N31" s="2"/>
       <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
+      <c r="P31" s="11"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="11"/>
+      <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
+      <c r="V31" s="11"/>
       <c r="W31" s="2"/>
-      <c r="X31" s="11"/>
+      <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
-    </row>
-    <row r="32" spans="1:26">
+      <c r="AA31" s="11"/>
+      <c r="AB31" s="2"/>
+      <c r="AC31" s="2"/>
+      <c r="AD31" s="42"/>
+      <c r="AE31" s="44"/>
+      <c r="AF31" s="44"/>
+      <c r="AG31" s="44"/>
+    </row>
+    <row r="32" spans="1:33">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="11"/>
+      <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="F32" s="11"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -2513,863 +2774,1087 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
-      <c r="N32" s="11"/>
+      <c r="N32" s="2"/>
       <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
+      <c r="P32" s="11"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="11"/>
+      <c r="S32" s="2"/>
       <c r="T32" s="2"/>
       <c r="U32" s="2"/>
-      <c r="V32" s="2"/>
+      <c r="V32" s="11"/>
       <c r="W32" s="2"/>
-      <c r="X32" s="11"/>
+      <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
-    </row>
-    <row r="33" spans="1:26">
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
+      <c r="AD32" s="42"/>
+      <c r="AE32" s="44"/>
+      <c r="AF32" s="44"/>
+      <c r="AG32" s="44"/>
+    </row>
+    <row r="33" spans="1:33">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="11"/>
+      <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="11"/>
       <c r="Q33" s="8"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="2"/>
+      <c r="R33" s="8"/>
+      <c r="S33" s="8"/>
+      <c r="T33" s="8"/>
       <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
+      <c r="V33" s="11"/>
       <c r="W33" s="2"/>
-      <c r="X33" s="11"/>
+      <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
-    </row>
-    <row r="34" spans="1:26">
+      <c r="AA33" s="11"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="42"/>
+      <c r="AE33" s="44"/>
+      <c r="AF33" s="44"/>
+      <c r="AG33" s="44"/>
+    </row>
+    <row r="34" spans="1:33">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="11"/>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="F34" s="11"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="11"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="N34" s="2"/>
       <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
+      <c r="P34" s="11"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-      <c r="S34" s="11"/>
+      <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
+      <c r="V34" s="11"/>
       <c r="W34" s="2"/>
-      <c r="X34" s="11"/>
+      <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
-    </row>
-    <row r="35" spans="1:26">
+      <c r="AA34" s="11"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="42"/>
+      <c r="AE34" s="44"/>
+      <c r="AF34" s="44"/>
+      <c r="AG34" s="44"/>
+    </row>
+    <row r="35" spans="1:33">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="11"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="F35" s="11"/>
       <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
-      <c r="N35" s="11"/>
+      <c r="N35" s="2"/>
       <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
+      <c r="P35" s="11"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-      <c r="S35" s="11"/>
+      <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
+      <c r="V35" s="11"/>
       <c r="W35" s="2"/>
-      <c r="X35" s="11"/>
+      <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
-    </row>
-    <row r="36" spans="1:26">
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="2"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="42"/>
+      <c r="AE35" s="44"/>
+      <c r="AF35" s="44"/>
+      <c r="AG35" s="44"/>
+    </row>
+    <row r="36" spans="1:33">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="11"/>
+      <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="F36" s="11"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="8"/>
+      <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="11"/>
+      <c r="M36" s="8"/>
+      <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
+      <c r="P36" s="11"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-      <c r="S36" s="11"/>
+      <c r="S36" s="2"/>
       <c r="T36" s="2"/>
       <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
+      <c r="V36" s="11"/>
       <c r="W36" s="2"/>
-      <c r="X36" s="11"/>
+      <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
-    </row>
-    <row r="37" spans="1:26">
+      <c r="AA36" s="11"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="42"/>
+      <c r="AE36" s="44"/>
+      <c r="AF36" s="44"/>
+      <c r="AG36" s="44"/>
+    </row>
+    <row r="37" spans="1:33">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="11"/>
+      <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
-      <c r="N37" s="11"/>
+      <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
+      <c r="P37" s="11"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
-      <c r="S37" s="11"/>
+      <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
+      <c r="V37" s="11"/>
       <c r="W37" s="2"/>
-      <c r="X37" s="11"/>
+      <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
-    </row>
-    <row r="38" spans="1:26">
+      <c r="AA37" s="11"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="42"/>
+      <c r="AE37" s="44"/>
+      <c r="AF37" s="44"/>
+      <c r="AG37" s="44"/>
+    </row>
+    <row r="38" spans="1:33">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="11"/>
+      <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="M38" s="8"/>
+      <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
+      <c r="P38" s="11"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
-      <c r="S38" s="11"/>
+      <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
-      <c r="V38" s="2"/>
+      <c r="V38" s="11"/>
       <c r="W38" s="2"/>
-      <c r="X38" s="11"/>
+      <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
-    </row>
-    <row r="39" spans="1:26">
+      <c r="AA38" s="11"/>
+      <c r="AB38" s="2"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="42"/>
+      <c r="AE38" s="44"/>
+      <c r="AF38" s="44"/>
+      <c r="AG38" s="44"/>
+    </row>
+    <row r="39" spans="1:33">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="11"/>
+      <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="F39" s="11"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="8"/>
       <c r="L39" s="2"/>
       <c r="M39" s="2"/>
-      <c r="N39" s="11"/>
+      <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
+      <c r="P39" s="11"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
-      <c r="S39" s="11"/>
+      <c r="S39" s="2"/>
       <c r="T39" s="2"/>
       <c r="U39" s="2"/>
-      <c r="V39" s="2"/>
+      <c r="V39" s="11"/>
       <c r="W39" s="2"/>
-      <c r="X39" s="11"/>
+      <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
-    </row>
-    <row r="40" spans="1:26">
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="2"/>
+      <c r="AC39" s="2"/>
+      <c r="AD39" s="42"/>
+      <c r="AE39" s="44"/>
+      <c r="AF39" s="44"/>
+      <c r="AG39" s="44"/>
+    </row>
+    <row r="40" spans="1:33">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="11"/>
+      <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
+      <c r="F40" s="11"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="8"/>
+      <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
+      <c r="K40" s="8"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
-      <c r="N40" s="11"/>
+      <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
+      <c r="P40" s="11"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
-      <c r="S40" s="11"/>
+      <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
-      <c r="V40" s="2"/>
+      <c r="V40" s="11"/>
       <c r="W40" s="2"/>
-      <c r="X40" s="11"/>
+      <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
-    </row>
-    <row r="41" spans="1:26">
+      <c r="AA40" s="11"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="42"/>
+      <c r="AE40" s="44"/>
+      <c r="AF40" s="44"/>
+      <c r="AG40" s="44"/>
+    </row>
+    <row r="41" spans="1:33">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="11"/>
+      <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="F41" s="11"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="P41" s="11"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
-      <c r="S41" s="11"/>
+      <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
+      <c r="V41" s="11"/>
       <c r="W41" s="2"/>
-      <c r="X41" s="11"/>
+      <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
-    </row>
-    <row r="42" spans="1:26">
+      <c r="AA41" s="11"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="42"/>
+      <c r="AE41" s="44"/>
+      <c r="AF41" s="44"/>
+      <c r="AG41" s="44"/>
+    </row>
+    <row r="42" spans="1:33">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="11"/>
+      <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="F42" s="11"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="15"/>
+      <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
+      <c r="J42" s="15"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
-      <c r="N42" s="11"/>
+      <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
+      <c r="P42" s="11"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
-      <c r="S42" s="11"/>
+      <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
-      <c r="V42" s="2"/>
+      <c r="V42" s="11"/>
       <c r="W42" s="2"/>
-      <c r="X42" s="11"/>
+      <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
-    </row>
-    <row r="43" spans="1:26">
+      <c r="AA42" s="11"/>
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="42"/>
+      <c r="AE42" s="44"/>
+      <c r="AF42" s="44"/>
+      <c r="AG42" s="44"/>
+    </row>
+    <row r="43" spans="1:33">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="15"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="19"/>
+      <c r="J43" s="15"/>
+      <c r="K43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="11"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="2"/>
       <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
+      <c r="P43" s="11"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-      <c r="S43" s="11"/>
+      <c r="S43" s="2"/>
       <c r="T43" s="2"/>
       <c r="U43" s="2"/>
-      <c r="V43" s="2"/>
+      <c r="V43" s="11"/>
       <c r="W43" s="2"/>
-      <c r="X43" s="11"/>
+      <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
-    </row>
-    <row r="44" spans="1:26">
+      <c r="AA43" s="11"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="42"/>
+      <c r="AE43" s="44"/>
+      <c r="AF43" s="44"/>
+      <c r="AG43" s="44"/>
+    </row>
+    <row r="44" spans="1:33">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="15"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="19"/>
+      <c r="J44" s="15"/>
+      <c r="K44" s="2"/>
       <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="11"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
+      <c r="P44" s="11"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
-      <c r="S44" s="11"/>
+      <c r="S44" s="2"/>
       <c r="T44" s="2"/>
       <c r="U44" s="2"/>
-      <c r="V44" s="2"/>
+      <c r="V44" s="11"/>
       <c r="W44" s="2"/>
-      <c r="X44" s="11"/>
+      <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
-    </row>
-    <row r="45" spans="1:26">
+      <c r="AA44" s="11"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="42"/>
+      <c r="AE44" s="44"/>
+      <c r="AF44" s="44"/>
+      <c r="AG44" s="44"/>
+    </row>
+    <row r="45" spans="1:33">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="15"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
+      <c r="J45" s="15"/>
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
-      <c r="N45" s="11"/>
+      <c r="N45" s="2"/>
       <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
+      <c r="P45" s="11"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-      <c r="S45" s="11"/>
+      <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="2"/>
-      <c r="V45" s="2"/>
+      <c r="V45" s="11"/>
       <c r="W45" s="2"/>
-      <c r="X45" s="11"/>
+      <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
-    </row>
-    <row r="46" spans="1:26">
+      <c r="AA45" s="11"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="42"/>
+      <c r="AE45" s="44"/>
+      <c r="AF45" s="44"/>
+      <c r="AG45" s="44"/>
+    </row>
+    <row r="46" spans="1:33">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="11"/>
+      <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
+      <c r="F46" s="11"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
-      <c r="L46" s="8"/>
+      <c r="L46" s="2"/>
       <c r="M46" s="2"/>
-      <c r="N46" s="11"/>
+      <c r="N46" s="8"/>
       <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
+      <c r="P46" s="11"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-      <c r="S46" s="11"/>
+      <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="2"/>
-      <c r="V46" s="2"/>
+      <c r="V46" s="11"/>
       <c r="W46" s="2"/>
-      <c r="X46" s="11"/>
+      <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
-    </row>
-    <row r="47" spans="1:26">
+      <c r="AA46" s="11"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="42"/>
+      <c r="AE46" s="44"/>
+      <c r="AF46" s="44"/>
+      <c r="AG46" s="44"/>
+    </row>
+    <row r="47" spans="1:33">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="11"/>
       <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
+      <c r="H47" s="2"/>
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="19"/>
+      <c r="K47" s="20"/>
+      <c r="L47" s="20"/>
       <c r="M47" s="2"/>
-      <c r="N47" s="11"/>
+      <c r="N47" s="19"/>
       <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
+      <c r="P47" s="11"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
-      <c r="S47" s="11"/>
+      <c r="S47" s="2"/>
       <c r="T47" s="2"/>
       <c r="U47" s="2"/>
-      <c r="V47" s="2"/>
+      <c r="V47" s="11"/>
       <c r="W47" s="2"/>
-      <c r="X47" s="11"/>
+      <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
-    </row>
-    <row r="48" spans="1:26">
+      <c r="AA47" s="11"/>
+      <c r="AB47" s="2"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="42"/>
+      <c r="AE47" s="44"/>
+      <c r="AF47" s="44"/>
+      <c r="AG47" s="44"/>
+    </row>
+    <row r="48" spans="1:33">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="11"/>
       <c r="G48" s="20"/>
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
-      <c r="K48" s="2"/>
-      <c r="L48" s="19"/>
+      <c r="K48" s="20"/>
+      <c r="L48" s="20"/>
       <c r="M48" s="2"/>
-      <c r="N48" s="11"/>
+      <c r="N48" s="19"/>
       <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
+      <c r="P48" s="11"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
-      <c r="S48" s="11"/>
+      <c r="S48" s="2"/>
       <c r="T48" s="2"/>
       <c r="U48" s="2"/>
-      <c r="V48" s="2"/>
+      <c r="V48" s="11"/>
       <c r="W48" s="2"/>
-      <c r="X48" s="11"/>
+      <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
-    </row>
-    <row r="49" spans="1:26">
+      <c r="AA48" s="11"/>
+      <c r="AB48" s="2"/>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="42"/>
+      <c r="AE48" s="44"/>
+      <c r="AF48" s="44"/>
+      <c r="AG48" s="44"/>
+    </row>
+    <row r="49" spans="1:33">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="11"/>
       <c r="G49" s="20"/>
-      <c r="H49" s="19"/>
+      <c r="H49" s="20"/>
       <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
       <c r="M49" s="2"/>
-      <c r="N49" s="11"/>
+      <c r="N49" s="19"/>
       <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
+      <c r="P49" s="11"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
-      <c r="S49" s="11"/>
+      <c r="S49" s="2"/>
       <c r="T49" s="2"/>
       <c r="U49" s="2"/>
-      <c r="V49" s="2"/>
+      <c r="V49" s="11"/>
       <c r="W49" s="2"/>
-      <c r="X49" s="11"/>
+      <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
-    </row>
-    <row r="50" spans="1:26">
+      <c r="AA49" s="11"/>
+      <c r="AB49" s="2"/>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="42"/>
+      <c r="AE49" s="44"/>
+      <c r="AF49" s="44"/>
+      <c r="AG49" s="44"/>
+    </row>
+    <row r="50" spans="1:33">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="11"/>
       <c r="G50" s="20"/>
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="19"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
       <c r="M50" s="2"/>
-      <c r="N50" s="11"/>
+      <c r="N50" s="19"/>
       <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
+      <c r="P50" s="11"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
-      <c r="S50" s="11"/>
+      <c r="S50" s="2"/>
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
-      <c r="V50" s="2"/>
+      <c r="V50" s="11"/>
       <c r="W50" s="2"/>
-      <c r="X50" s="11"/>
+      <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
-    </row>
-    <row r="51" spans="1:26">
+      <c r="AA50" s="11"/>
+      <c r="AB50" s="2"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="42"/>
+      <c r="AE50" s="44"/>
+      <c r="AF50" s="44"/>
+      <c r="AG50" s="44"/>
+    </row>
+    <row r="51" spans="1:33">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="11"/>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
-      <c r="I51" s="19"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="20"/>
+      <c r="I51" s="20"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
       <c r="M51" s="2"/>
-      <c r="N51" s="11"/>
+      <c r="N51" s="20"/>
       <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
+      <c r="P51" s="11"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
-      <c r="S51" s="11"/>
+      <c r="S51" s="2"/>
       <c r="T51" s="2"/>
       <c r="U51" s="2"/>
-      <c r="V51" s="2"/>
+      <c r="V51" s="11"/>
       <c r="W51" s="2"/>
-      <c r="X51" s="11"/>
+      <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
-    </row>
-    <row r="52" spans="1:26">
+      <c r="AA51" s="11"/>
+      <c r="AB51" s="2"/>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="42"/>
+      <c r="AE51" s="44"/>
+      <c r="AF51" s="44"/>
+      <c r="AG51" s="44"/>
+    </row>
+    <row r="52" spans="1:33">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="11"/>
       <c r="G52" s="20"/>
       <c r="H52" s="20"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
       <c r="M52" s="2"/>
-      <c r="N52" s="11"/>
+      <c r="N52" s="20"/>
       <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
+      <c r="P52" s="11"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
-      <c r="S52" s="11"/>
+      <c r="S52" s="2"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
+      <c r="V52" s="11"/>
       <c r="W52" s="2"/>
-      <c r="X52" s="11"/>
+      <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
-    </row>
-    <row r="53" spans="1:26">
+      <c r="AA52" s="11"/>
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="42"/>
+      <c r="AE52" s="44"/>
+      <c r="AF52" s="44"/>
+      <c r="AG52" s="44"/>
+    </row>
+    <row r="53" spans="1:33">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="11"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="11"/>
       <c r="H53" s="20"/>
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
-      <c r="K53" s="2"/>
+      <c r="K53" s="20"/>
       <c r="L53" s="20"/>
       <c r="M53" s="2"/>
-      <c r="N53" s="11"/>
+      <c r="N53" s="20"/>
       <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
+      <c r="P53" s="11"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
-      <c r="S53" s="11"/>
+      <c r="S53" s="2"/>
       <c r="T53" s="2"/>
       <c r="U53" s="2"/>
-      <c r="V53" s="2"/>
+      <c r="V53" s="11"/>
       <c r="W53" s="2"/>
-      <c r="X53" s="11"/>
+      <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
-    </row>
-    <row r="54" spans="1:26">
+      <c r="AA53" s="11"/>
+      <c r="AB53" s="2"/>
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="42"/>
+      <c r="AE53" s="44"/>
+      <c r="AF53" s="44"/>
+      <c r="AG53" s="44"/>
+    </row>
+    <row r="54" spans="1:33">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="11"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="11"/>
       <c r="H54" s="20"/>
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="21"/>
+      <c r="K54" s="20"/>
+      <c r="L54" s="20"/>
       <c r="M54" s="2"/>
-      <c r="N54" s="11"/>
+      <c r="N54" s="21"/>
       <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
+      <c r="P54" s="11"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
-      <c r="S54" s="11"/>
+      <c r="S54" s="2"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
+      <c r="V54" s="11"/>
       <c r="W54" s="2"/>
-      <c r="X54" s="11"/>
+      <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
-    </row>
-    <row r="55" spans="1:26">
+      <c r="AA54" s="11"/>
+      <c r="AB54" s="2"/>
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="42"/>
+      <c r="AE54" s="44"/>
+      <c r="AF54" s="44"/>
+      <c r="AG54" s="44"/>
+    </row>
+    <row r="55" spans="1:33">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="11"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="19"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="11"/>
+      <c r="H55" s="20"/>
       <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="2"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="20"/>
       <c r="L55" s="20"/>
       <c r="M55" s="2"/>
-      <c r="N55" s="11"/>
+      <c r="N55" s="20"/>
       <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
+      <c r="P55" s="11"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-      <c r="S55" s="11"/>
+      <c r="S55" s="2"/>
       <c r="T55" s="2"/>
       <c r="U55" s="2"/>
-      <c r="V55" s="2"/>
+      <c r="V55" s="11"/>
       <c r="W55" s="2"/>
-      <c r="X55" s="11"/>
+      <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
-    </row>
-    <row r="56" spans="1:26">
+      <c r="AA55" s="11"/>
+      <c r="AB55" s="2"/>
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="42"/>
+      <c r="AE55" s="44"/>
+      <c r="AF55" s="44"/>
+      <c r="AG55" s="44"/>
+    </row>
+    <row r="56" spans="1:33">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
-      <c r="D56" s="11"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="11"/>
       <c r="H56" s="20"/>
       <c r="I56" s="20"/>
       <c r="J56" s="20"/>
-      <c r="K56" s="2"/>
+      <c r="K56" s="20"/>
       <c r="L56" s="20"/>
       <c r="M56" s="2"/>
-      <c r="N56" s="11"/>
+      <c r="N56" s="20"/>
       <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
+      <c r="P56" s="11"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
-      <c r="S56" s="11"/>
+      <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
+      <c r="V56" s="11"/>
       <c r="W56" s="2"/>
-      <c r="X56" s="11"/>
+      <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
-    </row>
-    <row r="57" spans="1:26">
+      <c r="AA56" s="11"/>
+      <c r="AB56" s="2"/>
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="42"/>
+      <c r="AE56" s="44"/>
+      <c r="AF56" s="44"/>
+      <c r="AG56" s="44"/>
+    </row>
+    <row r="57" spans="1:33">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
-      <c r="D57" s="11"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="11"/>
+      <c r="H57" s="19"/>
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
-      <c r="K57" s="2"/>
+      <c r="K57" s="20"/>
       <c r="L57" s="20"/>
       <c r="M57" s="2"/>
-      <c r="N57" s="11"/>
+      <c r="N57" s="20"/>
       <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
+      <c r="P57" s="11"/>
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
-      <c r="S57" s="11"/>
+      <c r="S57" s="2"/>
       <c r="T57" s="2"/>
       <c r="U57" s="2"/>
-      <c r="V57" s="2"/>
+      <c r="V57" s="11"/>
       <c r="W57" s="2"/>
-      <c r="X57" s="11"/>
+      <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
-    </row>
-    <row r="58" spans="1:26">
+      <c r="AA57" s="11"/>
+      <c r="AB57" s="2"/>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="42"/>
+      <c r="AE57" s="44"/>
+      <c r="AF57" s="44"/>
+      <c r="AG57" s="44"/>
+    </row>
+    <row r="58" spans="1:33">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="11"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="20"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="11"/>
       <c r="H58" s="19"/>
       <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="2"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="20"/>
       <c r="L58" s="20"/>
       <c r="M58" s="2"/>
-      <c r="N58" s="11"/>
+      <c r="N58" s="20"/>
       <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
+      <c r="P58" s="11"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
-      <c r="S58" s="11"/>
+      <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
-      <c r="V58" s="2"/>
+      <c r="V58" s="11"/>
       <c r="W58" s="2"/>
-      <c r="X58" s="11"/>
+      <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
-    </row>
-    <row r="59" spans="1:26">
+      <c r="AA58" s="11"/>
+      <c r="AB58" s="2"/>
+      <c r="AC58" s="2"/>
+      <c r="AD58" s="42"/>
+      <c r="AE58" s="44"/>
+      <c r="AF58" s="44"/>
+      <c r="AG58" s="44"/>
+    </row>
+    <row r="59" spans="1:33">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="11"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="19"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="11"/>
+      <c r="H59" s="20"/>
       <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="2"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="20"/>
       <c r="L59" s="20"/>
       <c r="M59" s="2"/>
-      <c r="N59" s="11"/>
+      <c r="N59" s="20"/>
       <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
+      <c r="P59" s="11"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
-      <c r="S59" s="11"/>
+      <c r="S59" s="2"/>
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
+      <c r="V59" s="11"/>
       <c r="W59" s="2"/>
-      <c r="X59" s="11"/>
+      <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
-    </row>
-    <row r="60" spans="1:26">
+      <c r="AA59" s="11"/>
+      <c r="AB59" s="2"/>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="42"/>
+      <c r="AE59" s="44"/>
+      <c r="AF59" s="44"/>
+      <c r="AG59" s="44"/>
+    </row>
+    <row r="60" spans="1:33">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="11"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="19"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="11"/>
+      <c r="H60" s="20"/>
       <c r="I60" s="20"/>
-      <c r="J60" s="20"/>
-      <c r="K60" s="2"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="20"/>
       <c r="L60" s="20"/>
       <c r="M60" s="2"/>
-      <c r="N60" s="11"/>
+      <c r="N60" s="20"/>
       <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
+      <c r="P60" s="11"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
-      <c r="S60" s="11"/>
+      <c r="S60" s="2"/>
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
-      <c r="V60" s="2"/>
+      <c r="V60" s="11"/>
       <c r="W60" s="2"/>
-      <c r="X60" s="11"/>
+      <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
-    </row>
-    <row r="61" spans="1:26">
+      <c r="AA60" s="11"/>
+      <c r="AB60" s="2"/>
+      <c r="AC60" s="2"/>
+      <c r="AD60" s="42"/>
+      <c r="AE60" s="44"/>
+      <c r="AF60" s="44"/>
+      <c r="AG60" s="44"/>
+    </row>
+    <row r="61" spans="1:33">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
-      <c r="D61" s="11"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="11"/>
       <c r="H61" s="20"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
       <c r="M61" s="2"/>
-      <c r="N61" s="11"/>
+      <c r="N61" s="20"/>
       <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
+      <c r="P61" s="11"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
-      <c r="S61" s="11"/>
+      <c r="S61" s="2"/>
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
-      <c r="V61" s="2"/>
+      <c r="V61" s="11"/>
       <c r="W61" s="2"/>
-      <c r="X61" s="11"/>
+      <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
-    </row>
-    <row r="62" spans="1:26">
+      <c r="AA61" s="11"/>
+      <c r="AB61" s="2"/>
+      <c r="AC61" s="2"/>
+      <c r="AD61" s="42"/>
+      <c r="AE61" s="44"/>
+      <c r="AF61" s="44"/>
+      <c r="AG61" s="44"/>
+    </row>
+    <row r="62" spans="1:33">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="11"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="11"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
       <c r="M62" s="2"/>
-      <c r="N62" s="11"/>
+      <c r="N62" s="2"/>
       <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
+      <c r="P62" s="11"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
-      <c r="S62" s="11"/>
+      <c r="S62" s="2"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
-      <c r="V62" s="2"/>
+      <c r="V62" s="11"/>
       <c r="W62" s="2"/>
-      <c r="X62" s="11"/>
+      <c r="X62" s="2"/>
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
-    </row>
-    <row r="63" spans="1:26">
+      <c r="AA62" s="11"/>
+      <c r="AB62" s="2"/>
+      <c r="AC62" s="2"/>
+      <c r="AD62" s="42"/>
+      <c r="AE62" s="44"/>
+      <c r="AF62" s="44"/>
+      <c r="AG62" s="44"/>
+    </row>
+    <row r="63" spans="1:33">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
-      <c r="D63" s="11"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="11"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="11"/>
+      <c r="N63" s="2"/>
       <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
+      <c r="P63" s="11"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
-      <c r="S63" s="11"/>
+      <c r="S63" s="2"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
-      <c r="V63" s="2"/>
+      <c r="V63" s="11"/>
       <c r="W63" s="2"/>
-      <c r="X63" s="11"/>
+      <c r="X63" s="2"/>
       <c r="Y63" s="2"/>
       <c r="Z63" s="2"/>
+      <c r="AA63" s="11"/>
+      <c r="AB63" s="2"/>
+      <c r="AC63" s="2"/>
+      <c r="AD63" s="42"/>
+      <c r="AE63" s="44"/>
+      <c r="AF63" s="44"/>
+      <c r="AG63" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>